<commit_message>
improve codes for clean coding and improve question
</commit_message>
<xml_diff>
--- a/question.xlsx
+++ b/question.xlsx
@@ -61,6 +61,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">انتقال امتیاز امتیازی که برای دریافت وام با گردش حساب، معدل و </t>
     </r>
@@ -80,6 +81,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">به دست اومده رو میشه به نزدیکان انتقال داد</t>
     </r>
@@ -116,6 +118,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وام‌های خاص</t>
     </r>
@@ -135,6 +138,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ویژه</t>
     </r>
@@ -154,6 +158,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">بانک ملت </t>
     </r>
@@ -171,6 +176,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وام های ازدواج و فرزندآوری از وام‌های تکلیفی است که در این توصیه‌گر قرار ندارد</t>
     </r>
@@ -195,6 +201,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی است بدون ضامن که مشتریان دارای رتبه اعتباری </t>
     </r>
@@ -214,6 +221,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">و </t>
     </r>
@@ -233,6 +241,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">که اقدام به ثبت درخواست در سامانه فرابانک می‌نمایند، تا </t>
     </r>
@@ -252,6 +261,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">برابر معدل سه ماهه حساب‌های مجاز و تا سقف  ۱۰۰ میلیون تومان است</t>
     </r>
@@ -271,6 +281,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">دارابودن سایر شرایط احراز شامل نداشتن تعهدات غیرجاری و چک برگشتی الزامی است و حساب های مجاز برای دریافت وام، حساب های </t>
     </r>
@@ -290,6 +301,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">قرض الحسنه عادی، جاری و یا کوتاه مدت عادی است</t>
     </r>
@@ -309,6 +321,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">اعطای وام بدون ضامن </t>
     </r>
@@ -328,6 +341,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">بهان</t>
     </r>
@@ -347,8 +361,19 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">در سامانه فرابانک صرفاً به صورت غیرحضوری و با استفاده از برنامه کاربردی امضای ملت امکان‌پذیر است</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">در سامانه فرابانک صرفاً به صورت غیرحضوری و با استفاده از برنامه کاربردی امضای ملت امکان‌پذیر است. نرخ سود وام بهان ۲۳ درصد است</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">.</t>
     </r>
   </si>
   <si>
@@ -361,6 +386,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی است که مشتریان دارای رتبه اعتباری </t>
     </r>
@@ -380,6 +406,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">و </t>
     </r>
@@ -399,6 +426,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">و </t>
     </r>
@@ -418,6 +446,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">که اقدام به ثبت درخواست در سامانه فرابانک می‌نمایند تا </t>
     </r>
@@ -437,6 +466,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">برابر معدل سه ماهه حساب‌های مجاز و تا سقف مبلغی که سقف تسهیلات در فرابانک بر اساس رتبه اعتباری متقاضی تعیین می‌کند</t>
     </r>
@@ -456,6 +486,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">۲۰۰ میلیون تومان برای رتبه </t>
     </r>
@@ -475,6 +506,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">و ۱۵۰ میلیون تومان برای رتبه </t>
     </r>
@@ -494,6 +526,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">و ۱۰۰ میلیون تومان برای رتبه </t>
     </r>
@@ -513,6 +546,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">داده می‌شود</t>
     </r>
@@ -532,6 +566,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">دارابودن سایر شرایط احراز شامل نداشتن تعهدات غیرجاری و چک برگشتی الزامی است</t>
     </r>
@@ -551,6 +586,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">قابل ذکر است تنها به سپرده قرض الحسنه عادی، جاری و کوتاه مدت عادی این نوع تسهیلات تعلق می گیرد که می بایست حداقل </t>
     </r>
@@ -570,18 +606,29 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">ماه از زمان افتتاح حساب آن ها گذشته باشد</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="B Homa"/>
-        <family val="0"/>
-        <charset val="178"/>
-      </rPr>
-      <t xml:space="preserve">.</t>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">ماه از زمان افتتاح  حساب آن ها گذشته باشد</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="B Homa"/>
+        <family val="0"/>
+        <charset val="178"/>
+      </rPr>
+      <t xml:space="preserve">. نرخ سود وام فرابانک </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">۲۳ درصد است.</t>
     </r>
   </si>
   <si>
@@ -594,6 +641,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">نیازمند افتتاح حساب سپرده کوتاه مدت شایان یک می‌باشدو نیازمند ایجاد معدل حساب در میانگین </t>
     </r>
@@ -613,6 +661,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه، </t>
     </r>
@@ -632,6 +681,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه، </t>
     </r>
@@ -651,6 +701,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه و </t>
     </r>
@@ -670,6 +721,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه می‌باشد.
 در انواع عقد مرابحه، عقد جعاله و کارت اعتباری اعطا می‌شود. سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های مجاز برای دریافت وام </t>
@@ -690,6 +742,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -709,6 +762,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -728,6 +782,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -747,6 +802,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -758,7 +814,17 @@
         <family val="0"/>
         <charset val="178"/>
       </rPr>
-      <t xml:space="preserve">A است .تا مبلغ صد میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است.مشتریان دارای رتبه اعتباری D  و E که رتبه ایشان ناشی از شرایط و تعهدات غیرمستقیم است، می‌توانند در چارچوب ضوابط و مقررات جاری بانک از تسهیلات طرح شایان یک استفاده نمایند.</t>
+      <t xml:space="preserve">A است .تا مبلغ صد میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است.مشتریان دارای رتبه اعتباری D  و E که رتبه ایشان ناشی از شرایط و تعهدات غیرمستقیم است، می‌توانند در چارچوب ضوابط و مقررات جاری بانک از تسهیلات طرح شایان یک استفاده نمایند. نرخ سود وام شایان، </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">۱۴، ۱۸ و ۲۳ درصد است.</t>
     </r>
   </si>
   <si>
@@ -771,6 +837,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی که مشتریان به منظور برخورداری از مزایای طرح نیک وام باید حساب سپرده قرض‌الحسنه پس انداز نیک داشته باشند</t>
     </r>
@@ -790,6 +857,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">نیازمند ایجاد معدل حساب در میانگین </t>
     </r>
@@ -809,6 +877,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه، </t>
     </r>
@@ -828,6 +897,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه، </t>
     </r>
@@ -847,6 +917,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه و </t>
     </r>
@@ -866,6 +937,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه و </t>
     </r>
@@ -885,6 +957,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه می‌باشد</t>
     </r>
@@ -904,6 +977,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">سقف وام مبلغ ۳۰۰ میلیون تومان است و رتبه‌های مجاز برای دریافت وام </t>
     </r>
@@ -923,6 +997,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -942,6 +1017,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -961,6 +1037,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">است</t>
     </r>
@@ -980,6 +1057,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">شرط دریافت تسهیلات با دوره بازپرداخت </t>
     </r>
@@ -999,6 +1077,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">ماه داشتن رتبه </t>
     </r>
@@ -1018,6 +1097,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">یا </t>
     </r>
@@ -1037,6 +1117,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">برای متقاضی یا ضامن تسهیلات می باشد</t>
     </r>
@@ -1056,6 +1137,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">تا مبلغ صد میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است</t>
     </r>
@@ -1067,7 +1149,17 @@
         <family val="0"/>
         <charset val="178"/>
       </rPr>
-      <t xml:space="preserve">.</t>
+      <t xml:space="preserve">. نرخ سود وام نیک وام </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Noto Sans Devanagari"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">۴ درصد است.</t>
     </r>
   </si>
   <si>
@@ -1095,6 +1187,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی که مشتریان معرفی از سمت سازمان نظام مهندسی ساختمان استان تهران است و باید پروانه فعال سازمان نظام مهندسی ساختمان استان تهران داشته باشد</t>
     </r>
@@ -1114,6 +1207,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">رتبه‌های مجاز برای دریافت وام </t>
     </r>
@@ -1133,6 +1227,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -1152,6 +1247,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">،</t>
     </r>
@@ -1171,6 +1267,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">است و حساب های مجاز برای دریافت وام، حساب های سپرده قرض الحسنه عادی، جاری و سپرده کوتاه مدت هستند</t>
     </r>
@@ -1190,6 +1287,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">تا سقف ۱۰۰ میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است و سقف وام ۲۰۰ میلیون تومان با دوره بازپرداخت ۶۰ ماهه است</t>
     </r>
@@ -1214,6 +1312,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی است قرعه کشی که هر ۵ میلیون تومان در هر روز از هفتم تا بیست و ششم هر ماه، </t>
     </r>
@@ -1233,6 +1332,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">۵ میلیون تومان در هر روز از بیست و هفتم تا ششم ماه بعد، </t>
     </r>
@@ -1252,10 +1352,11 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">۵ میلیون تومان امتیاز تعلق می‌گیرد.
 برای محاسبه امتیاز در هر دوره قرعه‌کشی، همواره حداقل مانده روزانه دو ماه آخر در نظر گرفته می‌شود. حساب مجاز برای این وام، سپرده کوتاه مدت حقیقی انفرادی طرح گردونه است.
-قرعه‌کشی اواسط هر ماه است. در صورت برنده شدن حساب، امتیاز قبلی صفر و محاسبه امتیاز مجدد برای قرعه‌کشی بعدی از هفتم همان ماه است. حداقل ۵ میلیون تومان در بازه بیست و هفتم لغایت ششم ماه بعد در حساب طرح گردونه باید باشد. در صورتی‌که حتی یک روز در این بازه مانده حساب طرح گردونه از ۵ میلیون تومان  کمتر شود، حساب مشمول شرکت در قرعه‌کشی نیست. سقف وام ۳۰۰ میلیون تومان است. تا مبلغ ۲۰۰ میلیون تومان یک ضامن و بالاتر از این مبلغ دو ضامن الزامی است.</t>
+قرعه‌کشی اواسط هر ماه است. در صورت برنده شدن حساب، امتیاز قبلی صفر و محاسبه امتیاز مجدد برای قرعه‌کشی بعدی از هفتم همان ماه است. حداقل ۵ میلیون تومان در بازه بیست و هفتم لغایت ششم ماه بعد در حساب طرح گردونه باید باشد. در صورتی‌که حتی یک روز در این بازه مانده حساب طرح گردونه از ۵ میلیون تومان  کمتر شود، حساب مشمول شرکت در قرعه‌کشی نیست. سقف وام ۳۰۰ میلیون تومان است. تا مبلغ ۲۰۰ میلیون تومان یک ضامن و بالاتر از این مبلغ دو  ضامن الزامی است. نرخ سود وام گردونه ۴ درصد است.</t>
     </r>
   </si>
   <si>
@@ -1268,6 +1369,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">وامی بدون ضامن برای بازنشستگان آموزش و پرورش است</t>
     </r>
@@ -1287,6 +1389,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">حساب مجاز برای این وام، سپرده سرمایه‌‌گذاری یک‌ساله قلم است</t>
     </r>
@@ -1306,6 +1409,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">نرخ سود سالانه سپرده ۱۷ درصد است و نرخ سود وام ۱۶ درصد با تعداد اقساط ۴۸ ماهه است</t>
     </r>
@@ -1325,6 +1429,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">حداکثر مبلغ وام </t>
     </r>
@@ -1344,6 +1449,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">درصد مبلغ سپرده است</t>
     </r>
@@ -1368,6 +1474,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> وامی برای مشتریانی که حساب بانک ملت خود را به پایانه‌های فروش شرکت به‌پرداخت ملت متصل و رتبه لازم جهت گرفتن وام را دارند</t>
     </r>
@@ -1387,6 +1494,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">حساب‌های مجاز برای این وام، حساب‌های سپرده قرض الحسنه عادی، جاری ، سپرده کوتاه مدت ، بلند مدت و گواهی سپرده است</t>
     </r>
@@ -1406,6 +1514,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">مدل امتیازدهی، امتیاز پذیرنده نزد شعبه، برابر با مجموع امتیاز منابعی و تراکنشی است و  امتیاز منابعی، امتیاز کل پذیرنده، بر اساس معدل ماهیانه منابع مشتری نزد همان شعبه با ضرایب متناسب است و همچنین  امتیاز تراکنشی، مجموع ماهیانه مبالغ تراکنش تمامی پایانه‌های مشتری بر تعداد روزهای آن ماه تقسیم می‌شود</t>
     </r>
@@ -1425,6 +1534,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">رتبه پذیرندگی مشتری، بر اساس میانگین امتیاز کل کسب‌ شده توسط مشتری در سه ماه آخر است</t>
     </r>
@@ -1444,6 +1554,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">امتیاز هر مشتری در هر شعبه که دارای حساب متصل به پایانه فروش است، به صورت جداگانه محاسبه می‌شود</t>
     </r>
@@ -1468,6 +1579,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">استعلام رتبه اعتباری به فرآیندی اطلاق می‌شود که در آن وضعیت اعتباری یک فرد و  میزان ریسک اعتباری فرد بررسی می‌شود تا توانایی آن  در بازپرداخت بدهی‌ها ارزیابی شود</t>
     </r>
@@ -1487,6 +1599,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">این فرآیند در فرابانک توسط شرکت رتبه سنجی ایرانیان انجام می‌شود</t>
     </r>
@@ -1506,6 +1619,7 @@
         <color theme="1"/>
         <rFont val="Noto Sans Devanagari"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">حفظ رتبه اعتباری تا زمان دریافت تسهیلات الزامی بوده و در صورت کاهش امتیاز و رتبه اعتباری، امکان پرداخت تسهیلات وجود ندارد</t>
     </r>
@@ -1559,6 +1673,7 @@
       <color theme="1"/>
       <name val="Noto Sans Devanagari"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1631,48 +1746,44 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="2"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1870,205 +1981,205 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="58.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="91.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="58.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="91.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="4" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="6" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="17.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="132" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="76.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="4" t="s">
+    <row r="14" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="4" t="s">
+    <row r="15" customFormat="false" ht="90.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="60.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="4" t="s">
+    <row r="16" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8" t="s">
+      <c r="B16" s="9" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="157.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="9" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="60.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="B18" s="9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="114.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="4" t="s">
+    <row r="19" customFormat="false" ht="144.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="9" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="44" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="9" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="100.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="9" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="9" t="s">
+      <c r="A22" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="29.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="9" t="s">
+      <c r="A23" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>47</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit and imporve prompt and credit score detection
</commit_message>
<xml_diff>
--- a/question.xlsx
+++ b/question.xlsx
@@ -1981,8 +1981,8 @@
   </sheetPr>
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="true" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.68359375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2135,7 +2135,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="144.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="143.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>

</xml_diff>